<commit_message>
Updated Code for testing
</commit_message>
<xml_diff>
--- a/raw_data/original/Essay_Set_Descriptions/essay_set_descriptions.xlsx
+++ b/raw_data/original/Essay_Set_Descriptions/essay_set_descriptions.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_E1AE9A31E74D3462934AF85D1E929B2B29D20CC8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E0395BE-E21A-4C2B-9945-F822A0CF4DA1}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896"/>
+    <workbookView xWindow="32895" yWindow="10455" windowWidth="18735" windowHeight="10455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +77,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,6 +118,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -165,7 +169,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,9 +202,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,6 +254,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -408,17 +446,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="5" max="6" width="8.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>